<commit_message>
Revert "trying to refresh"
This reverts commit 5d80d7bb30a7ac6df956e41025c4019f45859698.
</commit_message>
<xml_diff>
--- a/phase_04/v1.6_finding_best_route/results/res_compiled.xlsx
+++ b/phase_04/v1.6_finding_best_route/results/res_compiled.xlsx
@@ -392,7 +392,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Desc</t>
   </si>
@@ -445,16 +445,13 @@
     <t>C</t>
   </si>
   <si>
-    <t xml:space="preserve">impute-all-&gt;obs-comb-&gt;all-params </t>
+    <t>impute-all-&gt;obs-comb-&gt;all-params (redo it)</t>
   </si>
   <si>
     <t>D</t>
   </si>
   <si>
     <t>obs-com-&gt;impute-all-&gt;all-params</t>
-  </si>
-  <si>
-    <t>impute-all-&gt;obs-comb-&gt;all-params , on redoig it</t>
   </si>
 </sst>
 </file>
@@ -1625,12 +1622,12 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.34074074074074" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="4.33333333333333" style="5" customWidth="1"/>
+    <col min="1" max="1" width="2.33333333333333" style="5" customWidth="1"/>
     <col min="2" max="2" width="37.3333333333333" style="5" customWidth="1"/>
     <col min="3" max="3" width="8.55555555555556" style="5" customWidth="1"/>
     <col min="4" max="4" width="8.88888888888889" style="5" customWidth="1"/>
@@ -2137,87 +2134,30 @@
       <c r="V9" s="16"/>
       <c r="W9" s="35"/>
     </row>
-    <row r="10" s="4" customFormat="1" ht="25.3" spans="1:32">
-      <c r="A10" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="19">
-        <v>66.72</v>
-      </c>
-      <c r="D10" s="19">
-        <v>2.3</v>
-      </c>
-      <c r="E10" s="19">
-        <v>63.6</v>
-      </c>
-      <c r="F10" s="19">
-        <v>70.9</v>
-      </c>
-      <c r="G10" s="19" t="str">
-        <f>_xlfn.DISPIMG("ID_56AA39F941CE4698B9CA85A7E550DCF9",1)</f>
-        <v>=DISPIMG("ID_56AA39F941CE4698B9CA85A7E550DCF9",1)</v>
-      </c>
-      <c r="H10" s="18">
-        <v>66.18</v>
-      </c>
-      <c r="I10" s="18">
-        <v>3.825</v>
-      </c>
-      <c r="J10" s="18">
-        <v>60</v>
-      </c>
-      <c r="K10" s="18">
-        <v>72.7</v>
-      </c>
-      <c r="L10" s="18" t="str">
-        <f>_xlfn.DISPIMG("ID_948E188BFA1242C8A2371B12BEC1C957",1)</f>
-        <v>=DISPIMG("ID_948E188BFA1242C8A2371B12BEC1C957",1)</v>
-      </c>
-      <c r="M10" s="28">
-        <v>72.2</v>
-      </c>
-      <c r="N10" s="29">
-        <v>1.2</v>
-      </c>
-      <c r="O10" s="29">
-        <v>70.9</v>
-      </c>
-      <c r="P10" s="29">
-        <v>74.54</v>
-      </c>
-      <c r="Q10" s="29" t="str">
-        <f>_xlfn.DISPIMG("ID_E74FC00E410F4AD3AC9FFB241A53A82E",1)</f>
-        <v>=DISPIMG("ID_E74FC00E410F4AD3AC9FFB241A53A82E",1)</v>
-      </c>
-      <c r="R10" s="18">
-        <v>68</v>
-      </c>
-      <c r="S10" s="18">
-        <v>2.87</v>
-      </c>
-      <c r="T10" s="18">
-        <v>65.45</v>
-      </c>
-      <c r="U10" s="18">
-        <v>72.72</v>
-      </c>
-      <c r="V10" s="18" t="str">
-        <f>_xlfn.DISPIMG("ID_20924FFC5B5544798BA400B31918271E",1)</f>
-        <v>=DISPIMG("ID_20924FFC5B5544798BA400B31918271E",1)</v>
-      </c>
-      <c r="W10" s="34"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="19"/>
-      <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
+    <row r="10" spans="1:23">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="35"/>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="15"/>

</xml_diff>